<commit_message>
Updated .xlsx file. Data reorganized to create graph
</commit_message>
<xml_diff>
--- a/Dataset2_info.xlsx
+++ b/Dataset2_info.xlsx
@@ -1,22 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tiziano/PycharmProjects/INFOMR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE3C796B-C86B-E144-8256-7EE6CD6AEB80}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CE2B81-AC9E-D740-BEF0-F20F2953F8F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="160" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset2_info" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">Dataset2_info!$L$2:$L$20</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">Dataset2_info!$N$1</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">Dataset2_info!$N$2:$N$20</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">Dataset2_info!$O$1</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">Dataset2_info!$O$2:$O$20</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">Dataset2_info!$P$1</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">Dataset2_info!$P$2:$P$20</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Dataset2_info!$M$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Dataset2_info!$M$2:$M$20</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="33">
   <si>
     <t>ID</t>
   </si>
@@ -110,6 +190,24 @@
   </si>
   <si>
     <t>Poly Av.</t>
+  </si>
+  <si>
+    <t>Avg # Vertexes</t>
+  </si>
+  <si>
+    <t>Avg # Faces</t>
+  </si>
+  <si>
+    <t>Max Vertexes</t>
+  </si>
+  <si>
+    <t>Min Vertexes</t>
+  </si>
+  <si>
+    <t>Max Faces</t>
+  </si>
+  <si>
+    <t>Min Faces</t>
   </si>
 </sst>
 </file>
@@ -702,8 +800,330 @@
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset2_info!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg # Vertexes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset2_info!$L$2:$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Airplane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Armadillo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bearing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bird</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bust</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cup</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FourLeg</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Glasses</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hand</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Mech</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Octopus</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plier</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Table</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Teddy</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Vase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset2_info!$M$2:$M$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>6350.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7480.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21077.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6402.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5395.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22003.55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10710.85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13696</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5999.15</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7615.65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4344.25</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7999.55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10113.049999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15054.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8847.0499999999993</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4678.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12848.1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12020.35</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11613.45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C30A-4740-875F-D4D951A3639D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset2_info!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max Vertexes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset2_info!$L$2:$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Airplane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Armadillo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bearing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bird</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bust</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cup</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FourLeg</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Glasses</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hand</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Mech</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Octopus</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plier</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Table</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Teddy</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Vase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset2_info!$N$2:$N$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>8679</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8640</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25494</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11790</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27824</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15246</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10186</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14680</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8771</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14084</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>15910</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19403</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15493</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6198</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15082</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>15169</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C30A-4740-875F-D4D951A3639D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -712,18 +1132,359 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="2068461439"/>
-        <c:axId val="2068376479"/>
+        <c:gapWidth val="269"/>
+        <c:axId val="1896437472"/>
+        <c:axId val="1837807296"/>
       </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset2_info!$O$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min Vertexes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset2_info!$L$2:$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Airplane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Armadillo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bearing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bird</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bust</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cup</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FourLeg</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Glasses</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hand</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Mech</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Octopus</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plier</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Table</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Teddy</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Vase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset2_info!$O$2:$O$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>5044</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5867</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1512</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2135</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5197</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5794</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6270</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1480</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1554</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1515</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2639</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11533</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1343</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3804</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9270</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9480</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3900</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C30A-4740-875F-D4D951A3639D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dataset2_info!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dataset2_info!$L$2:$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>Airplane</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Armadillo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Bearing</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bird</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Bust</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Chair</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Cup</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Fish</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>FourLeg</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Glasses</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Hand</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Human</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Mech</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Octopus</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Plier</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Table</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Teddy</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Vase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dataset2_info!$P$2:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10223.713157894737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C30A-4740-875F-D4D951A3639D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1896437472"/>
+        <c:axId val="1837807296"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="2068461439"/>
+        <c:axId val="1896437472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -760,7 +1521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2068376479"/>
+        <c:crossAx val="1837807296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -768,7 +1529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2068376479"/>
+        <c:axId val="1837807296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -788,6 +1549,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -818,7 +1580,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2068461439"/>
+        <c:crossAx val="1896437472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -830,6 +1592,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -915,7 +1708,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="322">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1240,8 +2033,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1305,6 +2098,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1423,23 +2227,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>151373</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>187037</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>269394</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>64142</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>618323</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>56701</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>413071</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>82358</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D27333B-3528-8846-B0E1-AA3A34CDEAD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC4D41D-BFFA-DE4D-A650-FB67B0496F17}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,15 +2561,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2198"/>
+  <dimension ref="A1:T2198"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1784,8 +2588,26 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>95</v>
       </c>
@@ -1801,8 +2623,35 @@
       <c r="E2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>6350.85</v>
+      </c>
+      <c r="N2">
+        <v>8679</v>
+      </c>
+      <c r="O2">
+        <v>5044</v>
+      </c>
+      <c r="P2">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q2">
+        <v>12697.7</v>
+      </c>
+      <c r="R2">
+        <v>17354</v>
+      </c>
+      <c r="S2">
+        <v>10084</v>
+      </c>
+      <c r="T2">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>81</v>
       </c>
@@ -1842,8 +2691,35 @@
         <f>MIN(D2:D21)</f>
         <v>11730</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3">
+        <v>7480.8</v>
+      </c>
+      <c r="N3">
+        <v>8640</v>
+      </c>
+      <c r="O3">
+        <v>5867</v>
+      </c>
+      <c r="P3">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q3">
+        <v>14957.8</v>
+      </c>
+      <c r="R3">
+        <v>17276</v>
+      </c>
+      <c r="S3">
+        <v>11730</v>
+      </c>
+      <c r="T3">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>94</v>
       </c>
@@ -1859,8 +2735,35 @@
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4">
+        <v>21077.25</v>
+      </c>
+      <c r="N4">
+        <v>25494</v>
+      </c>
+      <c r="O4">
+        <v>15000</v>
+      </c>
+      <c r="P4">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q4">
+        <v>42150.5</v>
+      </c>
+      <c r="R4">
+        <v>50984</v>
+      </c>
+      <c r="S4">
+        <v>29996</v>
+      </c>
+      <c r="T4">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>82</v>
       </c>
@@ -1876,8 +2779,35 @@
       <c r="E5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>19</v>
+      </c>
+      <c r="M5">
+        <v>6402.25</v>
+      </c>
+      <c r="N5">
+        <v>14994</v>
+      </c>
+      <c r="O5">
+        <v>1512</v>
+      </c>
+      <c r="P5">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q5">
+        <v>12803.3</v>
+      </c>
+      <c r="R5">
+        <v>29984</v>
+      </c>
+      <c r="S5">
+        <v>3020</v>
+      </c>
+      <c r="T5">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>96</v>
       </c>
@@ -1893,8 +2823,35 @@
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6">
+        <v>5395.55</v>
+      </c>
+      <c r="N6">
+        <v>11790</v>
+      </c>
+      <c r="O6">
+        <v>2135</v>
+      </c>
+      <c r="P6">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q6">
+        <v>10787.1</v>
+      </c>
+      <c r="R6">
+        <v>23576</v>
+      </c>
+      <c r="S6">
+        <v>4266</v>
+      </c>
+      <c r="T6">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>97</v>
       </c>
@@ -1910,8 +2867,35 @@
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7">
+        <v>22003.55</v>
+      </c>
+      <c r="N7">
+        <v>27824</v>
+      </c>
+      <c r="O7">
+        <v>5197</v>
+      </c>
+      <c r="P7">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q7">
+        <v>44003.1</v>
+      </c>
+      <c r="R7">
+        <v>55644</v>
+      </c>
+      <c r="S7">
+        <v>10390</v>
+      </c>
+      <c r="T7">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>83</v>
       </c>
@@ -1927,8 +2911,35 @@
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8">
+        <v>10710.85</v>
+      </c>
+      <c r="N8">
+        <v>15724</v>
+      </c>
+      <c r="O8">
+        <v>5794</v>
+      </c>
+      <c r="P8">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q8">
+        <v>21424.1</v>
+      </c>
+      <c r="R8">
+        <v>31456</v>
+      </c>
+      <c r="S8">
+        <v>11588</v>
+      </c>
+      <c r="T8">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>87</v>
       </c>
@@ -1944,8 +2955,35 @@
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>13696</v>
+      </c>
+      <c r="N9">
+        <v>15246</v>
+      </c>
+      <c r="O9">
+        <v>6270</v>
+      </c>
+      <c r="P9">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q9">
+        <v>27391.200000000001</v>
+      </c>
+      <c r="R9">
+        <v>30492</v>
+      </c>
+      <c r="S9">
+        <v>12540</v>
+      </c>
+      <c r="T9">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>93</v>
       </c>
@@ -1961,8 +2999,35 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10">
+        <v>5999.15</v>
+      </c>
+      <c r="N10">
+        <v>10186</v>
+      </c>
+      <c r="O10">
+        <v>4439</v>
+      </c>
+      <c r="P10">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q10">
+        <v>11994.3</v>
+      </c>
+      <c r="R10">
+        <v>20368</v>
+      </c>
+      <c r="S10">
+        <v>8874</v>
+      </c>
+      <c r="T10">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>92</v>
       </c>
@@ -1978,8 +3043,35 @@
       <c r="E11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11">
+        <v>7615.65</v>
+      </c>
+      <c r="N11">
+        <v>14680</v>
+      </c>
+      <c r="O11">
+        <v>1480</v>
+      </c>
+      <c r="P11">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q11">
+        <v>15227.3</v>
+      </c>
+      <c r="R11">
+        <v>29356</v>
+      </c>
+      <c r="S11">
+        <v>2956</v>
+      </c>
+      <c r="T11">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>86</v>
       </c>
@@ -1995,8 +3087,35 @@
       <c r="E12">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12">
+        <v>4344.25</v>
+      </c>
+      <c r="N12">
+        <v>8771</v>
+      </c>
+      <c r="O12">
+        <v>1554</v>
+      </c>
+      <c r="P12">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q12">
+        <v>8684.7000000000007</v>
+      </c>
+      <c r="R12">
+        <v>17538</v>
+      </c>
+      <c r="S12">
+        <v>3104</v>
+      </c>
+      <c r="T12">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>90</v>
       </c>
@@ -2012,8 +3131,35 @@
       <c r="E13">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" t="s">
+        <v>7</v>
+      </c>
+      <c r="M13">
+        <v>7999.55</v>
+      </c>
+      <c r="N13">
+        <v>14084</v>
+      </c>
+      <c r="O13">
+        <v>1515</v>
+      </c>
+      <c r="P13">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q13">
+        <v>15995.3</v>
+      </c>
+      <c r="R13">
+        <v>28164</v>
+      </c>
+      <c r="S13">
+        <v>3026</v>
+      </c>
+      <c r="T13">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>84</v>
       </c>
@@ -2029,8 +3175,35 @@
       <c r="E14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M14">
+        <v>10113.049999999999</v>
+      </c>
+      <c r="N14">
+        <v>15910</v>
+      </c>
+      <c r="O14">
+        <v>2639</v>
+      </c>
+      <c r="P14">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q14">
+        <v>20222.7</v>
+      </c>
+      <c r="R14">
+        <v>31816</v>
+      </c>
+      <c r="S14">
+        <v>5274</v>
+      </c>
+      <c r="T14">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>85</v>
       </c>
@@ -2046,8 +3219,35 @@
       <c r="E15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15">
+        <v>15054.1</v>
+      </c>
+      <c r="N15">
+        <v>19403</v>
+      </c>
+      <c r="O15">
+        <v>11533</v>
+      </c>
+      <c r="P15">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q15">
+        <v>30104.2</v>
+      </c>
+      <c r="R15">
+        <v>38802</v>
+      </c>
+      <c r="S15">
+        <v>23062</v>
+      </c>
+      <c r="T15">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>91</v>
       </c>
@@ -2063,8 +3263,35 @@
       <c r="E16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" t="s">
+        <v>17</v>
+      </c>
+      <c r="M16">
+        <v>8847.0499999999993</v>
+      </c>
+      <c r="N16">
+        <v>15493</v>
+      </c>
+      <c r="O16">
+        <v>1343</v>
+      </c>
+      <c r="P16">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q16">
+        <v>17690.5</v>
+      </c>
+      <c r="R16">
+        <v>30982</v>
+      </c>
+      <c r="S16">
+        <v>2682</v>
+      </c>
+      <c r="T16">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>88</v>
       </c>
@@ -2080,8 +3307,35 @@
       <c r="E17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <v>4678.75</v>
+      </c>
+      <c r="N17">
+        <v>6198</v>
+      </c>
+      <c r="O17">
+        <v>3804</v>
+      </c>
+      <c r="P17">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q17">
+        <v>9353.5</v>
+      </c>
+      <c r="R17">
+        <v>12392</v>
+      </c>
+      <c r="S17">
+        <v>7604</v>
+      </c>
+      <c r="T17">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>89</v>
       </c>
@@ -2097,8 +3351,35 @@
       <c r="E18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M18">
+        <v>12848.1</v>
+      </c>
+      <c r="N18">
+        <v>15082</v>
+      </c>
+      <c r="O18">
+        <v>9270</v>
+      </c>
+      <c r="P18">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q18">
+        <v>25692.2</v>
+      </c>
+      <c r="R18">
+        <v>30160</v>
+      </c>
+      <c r="S18">
+        <v>18536</v>
+      </c>
+      <c r="T18">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>99</v>
       </c>
@@ -2114,8 +3395,35 @@
       <c r="E19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" t="s">
+        <v>24</v>
+      </c>
+      <c r="M19">
+        <v>12020.35</v>
+      </c>
+      <c r="N19">
+        <v>15000</v>
+      </c>
+      <c r="O19">
+        <v>9480</v>
+      </c>
+      <c r="P19">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q19">
+        <v>24036.9</v>
+      </c>
+      <c r="R19">
+        <v>29996</v>
+      </c>
+      <c r="S19">
+        <v>18956</v>
+      </c>
+      <c r="T19">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>98</v>
       </c>
@@ -2131,8 +3439,35 @@
       <c r="E20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" t="s">
+        <v>11</v>
+      </c>
+      <c r="M20">
+        <v>11613.45</v>
+      </c>
+      <c r="N20">
+        <v>15169</v>
+      </c>
+      <c r="O20">
+        <v>3900</v>
+      </c>
+      <c r="P20">
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q20">
+        <v>23226.5</v>
+      </c>
+      <c r="R20">
+        <v>30342</v>
+      </c>
+      <c r="S20">
+        <v>7800</v>
+      </c>
+      <c r="T20">
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>100</v>
       </c>
@@ -2148,8 +3483,16 @@
       <c r="E21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <f>AVERAGE(M2:M20)</f>
+        <v>10223.713157894737</v>
+      </c>
+      <c r="Q21">
+        <f>AVERAGE(Q2:Q20)</f>
+        <v>20444.363157894739</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>194</v>
       </c>
@@ -2166,7 +3509,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>181</v>
       </c>
@@ -2207,7 +3550,7 @@
         <v>3026</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>195</v>
       </c>
@@ -2224,7 +3567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>183</v>
       </c>
@@ -2241,7 +3584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>197</v>
       </c>
@@ -2258,7 +3601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>196</v>
       </c>
@@ -2275,7 +3618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>182</v>
       </c>
@@ -2292,7 +3635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>186</v>
       </c>
@@ -2309,7 +3652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>192</v>
       </c>
@@ -2326,7 +3669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>193</v>
       </c>
@@ -2343,7 +3686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>187</v>
       </c>
@@ -39576,6 +40919,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L1:R2198">
+    <sortCondition ref="L1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>